<commit_message>
Changes for C and CAP
</commit_message>
<xml_diff>
--- a/EvoTax.1099/wwwroot/Templates/Form1099_CAP_Template.xlsx
+++ b/EvoTax.1099/wwwroot/Templates/Form1099_CAP_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://matthewjohnmcnally-my.sharepoint.com/personal/obaig_evolvedtax_com/Documents/Desktop/Excel sample/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Code Repos\EvoTaxes\EvoTax.1099\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_08A3CA524809CE4E5A6F2C93CEC19F165C90E916" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{172C290E-C76C-4761-9385-8E92A9BD0AA2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651C1F96-8259-4526-882E-8B64D156F2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="146">
   <si>
     <t>Rcp TIN</t>
   </si>
@@ -452,10 +452,13 @@
     <t>9.)  Fields in red font are required or the record will be rejected</t>
   </si>
   <si>
-    <t>Is Corrected</t>
-  </si>
-  <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Is Corrected Form of 1099</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1182,10 +1185,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1452,7 +1451,7 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V13"/>
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1545,7 +1544,7 @@
         <v>20</v>
       </c>
       <c r="V1" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
@@ -1601,7 +1600,7 @@
         <v>34</v>
       </c>
       <c r="V2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
@@ -1645,7 +1644,7 @@
         <v>33</v>
       </c>
       <c r="V3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
@@ -1689,7 +1688,7 @@
         <v>33</v>
       </c>
       <c r="V4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
@@ -1736,7 +1735,7 @@
         <v>57</v>
       </c>
       <c r="V5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
@@ -1780,7 +1779,7 @@
         <v>33</v>
       </c>
       <c r="V6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
@@ -1824,7 +1823,7 @@
         <v>33</v>
       </c>
       <c r="V7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
@@ -1874,7 +1873,7 @@
         <v>33</v>
       </c>
       <c r="V8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
@@ -1930,7 +1929,7 @@
         <v>40</v>
       </c>
       <c r="V9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
@@ -1980,7 +1979,7 @@
         <v>33</v>
       </c>
       <c r="V10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
@@ -2030,7 +2029,7 @@
         <v>33</v>
       </c>
       <c r="V11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
@@ -2083,7 +2082,7 @@
         <v>63</v>
       </c>
       <c r="V12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.35">
@@ -2124,12 +2123,12 @@
         <v>33</v>
       </c>
       <c r="V13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576" xr:uid="{6D70DFBC-1DD3-45EF-990F-EFFD01781E79}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576" xr:uid="{276CDD41-60F7-4411-B748-7E449BFF964B}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>